<commit_message>
small fix on the data files
</commit_message>
<xml_diff>
--- a/data/MSC/dcspt/PlanoCurso_9180_Planeamento Regional e Urbano.xlsx
+++ b/data/MSC/dcspt/PlanoCurso_9180_Planeamento Regional e Urbano.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/an/Library/CloudStorage/Dropbox/Toze/continUA/CE/levantamento CE/MSC/dcspt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uapt33090-my.sharepoint.com/personal/rita_almeida_ua_pt/Documents/Documents/Levantamento UCs Mestrado + CE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A988505-F104-2544-B2C3-5CFA63071804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CF96A80-32BA-4820-AD9D-FE58C5192FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{C8683CA5-2FB8-4AE0-98BD-BC01BAC8BBE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C8683CA5-2FB8-4AE0-98BD-BC01BAC8BBE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Consulta" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="108">
   <si>
     <t>DINÂMICAS SOCIO-ECONÓMICAS E TERRITORIAIS</t>
   </si>
@@ -330,6 +330,9 @@
     <t>Nº Total de Páginas: 1   (Num. Máx. Registos por Página: 150000)</t>
   </si>
   <si>
+    <t>Ramo 1- Desenvolvimento Local e Regional</t>
+  </si>
+  <si>
     <t>ESPAÇO PÚBLICO URBANO</t>
   </si>
   <si>
@@ -355,6 +358,9 @@
   </si>
   <si>
     <t>MOBILITY PLANNING</t>
+  </si>
+  <si>
+    <t>Ramo 2- Urbanismo</t>
   </si>
 </sst>
 </file>
@@ -407,12 +413,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -427,13 +439,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +467,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -768,236 +783,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129DAA54-F0CC-4470-9C3F-6928EBD02C11}">
-  <dimension ref="A1:AE41"/>
+  <dimension ref="A1:AE45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD24"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>47534</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2" t="s">
-        <v>5</v>
-      </c>
-      <c r="W2" t="s">
-        <v>6</v>
-      </c>
-      <c r="X2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>47734</v>
-      </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1075,15 +1009,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>47804</v>
+        <v>47734</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1161,15 +1095,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>47844</v>
+        <v>47804</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1247,15 +1181,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>48108</v>
+        <v>47844</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1315,13 +1249,13 @@
         <v>5</v>
       </c>
       <c r="W6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="Y6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -1333,36 +1267,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>42099</v>
+        <v>48108</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>6</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1380,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1401,13 +1335,13 @@
         <v>5</v>
       </c>
       <c r="W7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="X7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="Y7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -1419,15 +1353,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>47459</v>
+        <v>42099</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1466,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -1505,15 +1439,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>47735</v>
+        <v>47459</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1591,15 +1525,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>47812</v>
+        <v>47735</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1677,15 +1611,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>47822</v>
+        <v>47812</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1763,36 +1697,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>49991</v>
+        <v>47822</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I12">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1804,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1828,7 +1762,16 @@
         <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="W12" t="s">
+        <v>6</v>
+      </c>
+      <c r="X12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>8</v>
       </c>
       <c r="Z12">
         <v>0</v>
@@ -1840,36 +1783,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>49904</v>
+        <v>49991</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="I13">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1917,15 +1860,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>42100</v>
+        <v>49904</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1958,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1982,25 +1925,10 @@
         <v>0</v>
       </c>
       <c r="V14" t="s">
-        <v>5</v>
-      </c>
-      <c r="W14" t="s">
-        <v>6</v>
-      </c>
-      <c r="X14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="Z14">
-        <v>49904</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -2009,15 +1937,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>47853</v>
+        <v>42100</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -2041,10 +1969,10 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -2077,13 +2005,13 @@
         <v>5</v>
       </c>
       <c r="W15" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="X15" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="Y15" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="Z15">
         <v>49904</v>
@@ -2101,15 +2029,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>45658</v>
+        <v>47853</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -2133,10 +2061,10 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L16" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2169,13 +2097,13 @@
         <v>5</v>
       </c>
       <c r="W16" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="X16" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="Y16" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="Z16">
         <v>49904</v>
@@ -2193,15 +2121,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>47817</v>
+        <v>45658</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2285,15 +2213,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>47564</v>
+        <v>47817</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -2317,10 +2245,10 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -2353,13 +2281,13 @@
         <v>5</v>
       </c>
       <c r="W18" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="X18" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="Y18" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="Z18">
         <v>49904</v>
@@ -2377,15 +2305,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>47741</v>
+        <v>47564</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -2409,10 +2337,10 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L19" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -2469,15 +2397,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>47527</v>
+        <v>47741</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -2501,10 +2429,10 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -2537,13 +2465,13 @@
         <v>5</v>
       </c>
       <c r="W20" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="X20" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="Y20" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="Z20">
         <v>49904</v>
@@ -2561,95 +2489,110 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>47527</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21" t="s">
+        <v>5</v>
+      </c>
+      <c r="W21" t="s">
+        <v>56</v>
+      </c>
+      <c r="X21" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z21">
+        <v>49904</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>49990</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>59</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>6</v>
-      </c>
-      <c r="I21">
-        <v>6</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AD21">
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>47534</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
         <v>2</v>
@@ -2679,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -2703,1673 +2646,1905 @@
         <v>0</v>
       </c>
       <c r="V22" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="S25" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="T25" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="U25" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="V25" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="W25" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="X25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y25" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z25" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA25" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB25" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE25" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>47534</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7">
+        <v>6</v>
+      </c>
+      <c r="I26" s="7">
+        <v>6</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7">
+        <v>1</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="7">
+        <v>0</v>
+      </c>
+      <c r="N26" s="7">
+        <v>3</v>
+      </c>
+      <c r="O26" s="7">
+        <v>0</v>
+      </c>
+      <c r="P26" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>0</v>
+      </c>
+      <c r="R26" s="7">
+        <v>0</v>
+      </c>
+      <c r="S26" s="7">
+        <v>0</v>
+      </c>
+      <c r="T26" s="7">
+        <v>0</v>
+      </c>
+      <c r="U26" s="7">
+        <v>0</v>
+      </c>
+      <c r="V26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W22" t="s">
-        <v>6</v>
-      </c>
-      <c r="X22" t="s">
+      <c r="W26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Y26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AD22">
-        <v>0</v>
-      </c>
-      <c r="AE22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="Z26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>47567</v>
       </c>
-      <c r="B23" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B27" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>6</v>
-      </c>
-      <c r="I23">
-        <v>6</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="C27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7">
+        <v>6</v>
+      </c>
+      <c r="I27" s="7">
+        <v>6</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0</v>
+      </c>
+      <c r="K27" s="7">
+        <v>1</v>
+      </c>
+      <c r="L27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>3</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23" t="s">
+      <c r="M27" s="7">
+        <v>0</v>
+      </c>
+      <c r="N27" s="7">
+        <v>3</v>
+      </c>
+      <c r="O27" s="7">
+        <v>0</v>
+      </c>
+      <c r="P27" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>0</v>
+      </c>
+      <c r="R27" s="7">
+        <v>0</v>
+      </c>
+      <c r="S27" s="7">
+        <v>0</v>
+      </c>
+      <c r="T27" s="7">
+        <v>0</v>
+      </c>
+      <c r="U27" s="7">
+        <v>0</v>
+      </c>
+      <c r="V27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W23" t="s">
-        <v>6</v>
-      </c>
-      <c r="X23" t="s">
+      <c r="W27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X27" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Y27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z23">
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <v>0</v>
-      </c>
-      <c r="AE23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="Z27" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="7"/>
+      <c r="AD27" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>47590</v>
       </c>
-      <c r="B24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B28" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>6</v>
-      </c>
-      <c r="I24">
-        <v>6</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="C28" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="7">
+        <v>1</v>
+      </c>
+      <c r="H28" s="7">
+        <v>6</v>
+      </c>
+      <c r="I28" s="7">
+        <v>6</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <v>1</v>
+      </c>
+      <c r="L28" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>3</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-      <c r="V24" t="s">
-        <v>101</v>
-      </c>
-      <c r="W24" t="s">
-        <v>6</v>
-      </c>
-      <c r="X24" t="s">
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
+        <v>3</v>
+      </c>
+      <c r="O28" s="7">
+        <v>0</v>
+      </c>
+      <c r="P28" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0</v>
+      </c>
+      <c r="R28" s="7">
+        <v>0</v>
+      </c>
+      <c r="S28" s="7">
+        <v>0</v>
+      </c>
+      <c r="T28" s="7">
+        <v>0</v>
+      </c>
+      <c r="U28" s="7">
+        <v>0</v>
+      </c>
+      <c r="V28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Y28" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z24">
-        <v>0</v>
-      </c>
-      <c r="AD24">
-        <v>0</v>
-      </c>
-      <c r="AE24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="Z28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="7"/>
+      <c r="AB28" s="7"/>
+      <c r="AC28" s="7"/>
+      <c r="AD28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>47734</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>6</v>
-      </c>
-      <c r="I25">
-        <v>6</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+      <c r="H29" s="7">
+        <v>6</v>
+      </c>
+      <c r="I29" s="7">
+        <v>6</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1</v>
+      </c>
+      <c r="L29" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>3</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
-      <c r="V25" t="s">
+      <c r="M29" s="7">
+        <v>0</v>
+      </c>
+      <c r="N29" s="7">
+        <v>3</v>
+      </c>
+      <c r="O29" s="7">
+        <v>0</v>
+      </c>
+      <c r="P29" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>0</v>
+      </c>
+      <c r="R29" s="7">
+        <v>0</v>
+      </c>
+      <c r="S29" s="7">
+        <v>0</v>
+      </c>
+      <c r="T29" s="7">
+        <v>0</v>
+      </c>
+      <c r="U29" s="7">
+        <v>0</v>
+      </c>
+      <c r="V29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W25" t="s">
-        <v>6</v>
-      </c>
-      <c r="X25" t="s">
+      <c r="W29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X29" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Y29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z25">
-        <v>0</v>
-      </c>
-      <c r="AD25">
-        <v>0</v>
-      </c>
-      <c r="AE25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="Z29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
+      <c r="AC29" s="7"/>
+      <c r="AD29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>47804</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B30" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <v>6</v>
-      </c>
-      <c r="I26">
-        <v>6</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7">
+        <v>6</v>
+      </c>
+      <c r="I30" s="7">
+        <v>6</v>
+      </c>
+      <c r="J30" s="7">
+        <v>0</v>
+      </c>
+      <c r="K30" s="7">
+        <v>1</v>
+      </c>
+      <c r="L30" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>3</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-      <c r="V26" t="s">
+      <c r="M30" s="7">
+        <v>0</v>
+      </c>
+      <c r="N30" s="7">
+        <v>3</v>
+      </c>
+      <c r="O30" s="7">
+        <v>0</v>
+      </c>
+      <c r="P30" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>0</v>
+      </c>
+      <c r="R30" s="7">
+        <v>0</v>
+      </c>
+      <c r="S30" s="7">
+        <v>0</v>
+      </c>
+      <c r="T30" s="7">
+        <v>0</v>
+      </c>
+      <c r="U30" s="7">
+        <v>0</v>
+      </c>
+      <c r="V30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W26" t="s">
-        <v>6</v>
-      </c>
-      <c r="X26" t="s">
+      <c r="W30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X30" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Y30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AD26">
-        <v>0</v>
-      </c>
-      <c r="AE26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="Z30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>42101</v>
       </c>
-      <c r="B27" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B31" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="C31" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F31" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="H27">
-        <v>6</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>6</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="G31" s="7">
+        <v>2</v>
+      </c>
+      <c r="H31" s="7">
+        <v>6</v>
+      </c>
+      <c r="I31" s="7">
+        <v>0</v>
+      </c>
+      <c r="J31" s="7">
+        <v>6</v>
+      </c>
+      <c r="K31" s="7">
+        <v>1</v>
+      </c>
+      <c r="L31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>3</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27" t="s">
+      <c r="M31" s="7">
+        <v>0</v>
+      </c>
+      <c r="N31" s="7">
+        <v>3</v>
+      </c>
+      <c r="O31" s="7">
+        <v>0</v>
+      </c>
+      <c r="P31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>0</v>
+      </c>
+      <c r="R31" s="7">
+        <v>0</v>
+      </c>
+      <c r="S31" s="7">
+        <v>0</v>
+      </c>
+      <c r="T31" s="7">
+        <v>0</v>
+      </c>
+      <c r="U31" s="7">
+        <v>0</v>
+      </c>
+      <c r="V31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W27" t="s">
-        <v>6</v>
-      </c>
-      <c r="X27" t="s">
+      <c r="W31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Y31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z27">
-        <v>0</v>
-      </c>
-      <c r="AD27">
-        <v>0</v>
-      </c>
-      <c r="AE27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="Z31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>47732</v>
       </c>
-      <c r="B28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B32" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="C32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="H28">
-        <v>6</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>6</v>
-      </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="G32" s="7">
+        <v>2</v>
+      </c>
+      <c r="H32" s="7">
+        <v>6</v>
+      </c>
+      <c r="I32" s="7">
+        <v>0</v>
+      </c>
+      <c r="J32" s="7">
+        <v>6</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="L32" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>3</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="T28">
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
-      <c r="V28" t="s">
+      <c r="M32" s="7">
+        <v>0</v>
+      </c>
+      <c r="N32" s="7">
+        <v>3</v>
+      </c>
+      <c r="O32" s="7">
+        <v>0</v>
+      </c>
+      <c r="P32" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>0</v>
+      </c>
+      <c r="R32" s="7">
+        <v>0</v>
+      </c>
+      <c r="S32" s="7">
+        <v>0</v>
+      </c>
+      <c r="T32" s="7">
+        <v>0</v>
+      </c>
+      <c r="U32" s="7">
+        <v>0</v>
+      </c>
+      <c r="V32" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W28" t="s">
-        <v>6</v>
-      </c>
-      <c r="X28" t="s">
+      <c r="W32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Y32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z28">
-        <v>0</v>
-      </c>
-      <c r="AD28">
-        <v>0</v>
-      </c>
-      <c r="AE28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="Z32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>47735</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C33" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F33" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G29">
-        <v>2</v>
-      </c>
-      <c r="H29">
-        <v>6</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>6</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="G33" s="7">
+        <v>2</v>
+      </c>
+      <c r="H33" s="7">
+        <v>6</v>
+      </c>
+      <c r="I33" s="7">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7">
+        <v>6</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+      <c r="L33" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>3</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-      <c r="V29" t="s">
+      <c r="M33" s="7">
+        <v>0</v>
+      </c>
+      <c r="N33" s="7">
+        <v>3</v>
+      </c>
+      <c r="O33" s="7">
+        <v>0</v>
+      </c>
+      <c r="P33" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>0</v>
+      </c>
+      <c r="R33" s="7">
+        <v>0</v>
+      </c>
+      <c r="S33" s="7">
+        <v>0</v>
+      </c>
+      <c r="T33" s="7">
+        <v>0</v>
+      </c>
+      <c r="U33" s="7">
+        <v>0</v>
+      </c>
+      <c r="V33" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W29" t="s">
-        <v>6</v>
-      </c>
-      <c r="X29" t="s">
+      <c r="W33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Y33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z29">
-        <v>0</v>
-      </c>
-      <c r="AD29">
-        <v>0</v>
-      </c>
-      <c r="AE29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="Z33" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>47812</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B34" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G30">
-        <v>2</v>
-      </c>
-      <c r="H30">
-        <v>6</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>6</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="G34" s="7">
+        <v>2</v>
+      </c>
+      <c r="H34" s="7">
+        <v>6</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0</v>
+      </c>
+      <c r="J34" s="7">
+        <v>6</v>
+      </c>
+      <c r="K34" s="7">
+        <v>1</v>
+      </c>
+      <c r="L34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <v>3</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <v>0</v>
-      </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
-      <c r="T30">
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <v>0</v>
-      </c>
-      <c r="V30" t="s">
+      <c r="M34" s="7">
+        <v>0</v>
+      </c>
+      <c r="N34" s="7">
+        <v>3</v>
+      </c>
+      <c r="O34" s="7">
+        <v>0</v>
+      </c>
+      <c r="P34" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>0</v>
+      </c>
+      <c r="R34" s="7">
+        <v>0</v>
+      </c>
+      <c r="S34" s="7">
+        <v>0</v>
+      </c>
+      <c r="T34" s="7">
+        <v>0</v>
+      </c>
+      <c r="U34" s="7">
+        <v>0</v>
+      </c>
+      <c r="V34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W30" t="s">
-        <v>6</v>
-      </c>
-      <c r="X30" t="s">
+      <c r="W34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X34" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Y34" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z30">
-        <v>0</v>
-      </c>
-      <c r="AD30">
-        <v>0</v>
-      </c>
-      <c r="AE30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="Z34" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>47822</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C35" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D35" s="7">
+        <v>1</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="H31">
-        <v>6</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>6</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="G35" s="7">
+        <v>2</v>
+      </c>
+      <c r="H35" s="7">
+        <v>6</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0</v>
+      </c>
+      <c r="J35" s="7">
+        <v>6</v>
+      </c>
+      <c r="K35" s="7">
+        <v>1</v>
+      </c>
+      <c r="L35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>3</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-      <c r="V31" t="s">
+      <c r="M35" s="7">
+        <v>0</v>
+      </c>
+      <c r="N35" s="7">
+        <v>3</v>
+      </c>
+      <c r="O35" s="7">
+        <v>0</v>
+      </c>
+      <c r="P35" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>0</v>
+      </c>
+      <c r="R35" s="7">
+        <v>0</v>
+      </c>
+      <c r="S35" s="7">
+        <v>0</v>
+      </c>
+      <c r="T35" s="7">
+        <v>0</v>
+      </c>
+      <c r="U35" s="7">
+        <v>0</v>
+      </c>
+      <c r="V35" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W31" t="s">
-        <v>6</v>
-      </c>
-      <c r="X31" t="s">
+      <c r="W35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X35" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Y35" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z31">
-        <v>0</v>
-      </c>
-      <c r="AD31">
-        <v>0</v>
-      </c>
-      <c r="AE31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="Z35" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>49991</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B36" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C36" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D36" s="7">
+        <v>2</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
         <v>48</v>
       </c>
-      <c r="I32">
+      <c r="I36" s="7">
         <v>18</v>
       </c>
-      <c r="J32">
+      <c r="J36" s="7">
         <v>30</v>
       </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32" t="s">
+      <c r="K36" s="7">
+        <v>1</v>
+      </c>
+      <c r="L36" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M32">
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
-      <c r="V32" t="s">
+      <c r="M36" s="7">
+        <v>0</v>
+      </c>
+      <c r="N36" s="7">
+        <v>0</v>
+      </c>
+      <c r="O36" s="7">
+        <v>0</v>
+      </c>
+      <c r="P36" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0</v>
+      </c>
+      <c r="R36" s="7">
+        <v>0</v>
+      </c>
+      <c r="S36" s="7">
+        <v>0</v>
+      </c>
+      <c r="T36" s="7">
+        <v>0</v>
+      </c>
+      <c r="U36" s="7">
+        <v>0</v>
+      </c>
+      <c r="V36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Z32">
-        <v>0</v>
-      </c>
-      <c r="AD32">
-        <v>0</v>
-      </c>
-      <c r="AE32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>49904</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C37" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <v>6</v>
-      </c>
-      <c r="I33">
-        <v>6</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="D37" s="7">
+        <v>2</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7">
+        <v>6</v>
+      </c>
+      <c r="I37" s="7">
+        <v>6</v>
+      </c>
+      <c r="J37" s="7">
+        <v>0</v>
+      </c>
+      <c r="K37" s="7">
+        <v>1</v>
+      </c>
+      <c r="L37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
-      <c r="T33">
-        <v>0</v>
-      </c>
-      <c r="U33">
-        <v>0</v>
-      </c>
-      <c r="V33" t="s">
+      <c r="M37" s="7">
+        <v>0</v>
+      </c>
+      <c r="N37" s="7">
+        <v>0</v>
+      </c>
+      <c r="O37" s="7">
+        <v>0</v>
+      </c>
+      <c r="P37" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>0</v>
+      </c>
+      <c r="R37" s="7">
+        <v>0</v>
+      </c>
+      <c r="S37" s="7">
+        <v>0</v>
+      </c>
+      <c r="T37" s="7">
+        <v>0</v>
+      </c>
+      <c r="U37" s="7">
+        <v>0</v>
+      </c>
+      <c r="V37" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Z33">
-        <v>0</v>
-      </c>
-      <c r="AD33">
-        <v>0</v>
-      </c>
-      <c r="AE33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>47817</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C38" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>2</v>
-      </c>
-      <c r="F34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>6</v>
-      </c>
-      <c r="I34">
-        <v>6</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="D38" s="7">
+        <v>2</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1</v>
+      </c>
+      <c r="H38" s="7">
+        <v>6</v>
+      </c>
+      <c r="I38" s="7">
+        <v>6</v>
+      </c>
+      <c r="J38" s="7">
+        <v>0</v>
+      </c>
+      <c r="K38" s="7">
+        <v>1</v>
+      </c>
+      <c r="L38" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <v>3</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <v>0</v>
-      </c>
-      <c r="S34">
-        <v>0</v>
-      </c>
-      <c r="T34">
-        <v>0</v>
-      </c>
-      <c r="U34">
-        <v>0</v>
-      </c>
-      <c r="V34" t="s">
+      <c r="M38" s="7">
+        <v>0</v>
+      </c>
+      <c r="N38" s="7">
+        <v>3</v>
+      </c>
+      <c r="O38" s="7">
+        <v>0</v>
+      </c>
+      <c r="P38" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="7">
+        <v>0</v>
+      </c>
+      <c r="R38" s="7">
+        <v>0</v>
+      </c>
+      <c r="S38" s="7">
+        <v>0</v>
+      </c>
+      <c r="T38" s="7">
+        <v>0</v>
+      </c>
+      <c r="U38" s="7">
+        <v>0</v>
+      </c>
+      <c r="V38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="X34" t="s">
+      <c r="X38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Y38" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Z34">
+      <c r="Z38" s="7">
         <v>49904</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AA38" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AB38" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AD34">
-        <v>0</v>
-      </c>
-      <c r="AE34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>47564</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B39" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C39" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>6</v>
-      </c>
-      <c r="I35">
-        <v>6</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
+      <c r="D39" s="7">
+        <v>2</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="7">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7">
+        <v>6</v>
+      </c>
+      <c r="I39" s="7">
+        <v>6</v>
+      </c>
+      <c r="J39" s="7">
+        <v>0</v>
+      </c>
+      <c r="K39" s="7">
         <v>5</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L39" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <v>3</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>0</v>
-      </c>
-      <c r="S35">
-        <v>0</v>
-      </c>
-      <c r="T35">
-        <v>0</v>
-      </c>
-      <c r="U35">
-        <v>0</v>
-      </c>
-      <c r="V35" t="s">
+      <c r="M39" s="7">
+        <v>0</v>
+      </c>
+      <c r="N39" s="7">
+        <v>3</v>
+      </c>
+      <c r="O39" s="7">
+        <v>0</v>
+      </c>
+      <c r="P39" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="7">
+        <v>0</v>
+      </c>
+      <c r="R39" s="7">
+        <v>0</v>
+      </c>
+      <c r="S39" s="7">
+        <v>0</v>
+      </c>
+      <c r="T39" s="7">
+        <v>0</v>
+      </c>
+      <c r="U39" s="7">
+        <v>0</v>
+      </c>
+      <c r="V39" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W35" t="s">
-        <v>6</v>
-      </c>
-      <c r="X35" t="s">
+      <c r="W39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Y39" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z35">
+      <c r="Z39" s="7">
         <v>49904</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AA39" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AB35" t="s">
+      <c r="AB39" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AD35">
-        <v>0</v>
-      </c>
-      <c r="AE35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>47527</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B40" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C40" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36">
-        <v>6</v>
-      </c>
-      <c r="I36">
-        <v>6</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
+      <c r="D40" s="7">
+        <v>2</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1</v>
+      </c>
+      <c r="H40" s="7">
+        <v>6</v>
+      </c>
+      <c r="I40" s="7">
+        <v>6</v>
+      </c>
+      <c r="J40" s="7">
+        <v>0</v>
+      </c>
+      <c r="K40" s="7">
         <v>5</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L40" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <v>3</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
-      <c r="S36">
-        <v>0</v>
-      </c>
-      <c r="T36">
-        <v>0</v>
-      </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-      <c r="V36" t="s">
+      <c r="M40" s="7">
+        <v>0</v>
+      </c>
+      <c r="N40" s="7">
+        <v>3</v>
+      </c>
+      <c r="O40" s="7">
+        <v>0</v>
+      </c>
+      <c r="P40" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>0</v>
+      </c>
+      <c r="R40" s="7">
+        <v>0</v>
+      </c>
+      <c r="S40" s="7">
+        <v>0</v>
+      </c>
+      <c r="T40" s="7">
+        <v>0</v>
+      </c>
+      <c r="U40" s="7">
+        <v>0</v>
+      </c>
+      <c r="V40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W36" t="s">
+      <c r="W40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="X36" t="s">
+      <c r="X40" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Y40" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="Z36">
+      <c r="Z40" s="7">
         <v>49904</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AA40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AB36" t="s">
+      <c r="AB40" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AD36">
-        <v>0</v>
-      </c>
-      <c r="AE36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="AC40" s="7"/>
+      <c r="AD40" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>45658</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C41" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
-        <v>6</v>
-      </c>
-      <c r="I37">
-        <v>6</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="D41" s="7">
+        <v>2</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1</v>
+      </c>
+      <c r="H41" s="7">
+        <v>6</v>
+      </c>
+      <c r="I41" s="7">
+        <v>6</v>
+      </c>
+      <c r="J41" s="7">
+        <v>0</v>
+      </c>
+      <c r="K41" s="7">
+        <v>1</v>
+      </c>
+      <c r="L41" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <v>3</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="R37">
-        <v>0</v>
-      </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
-      <c r="V37" t="s">
+      <c r="M41" s="7">
+        <v>0</v>
+      </c>
+      <c r="N41" s="7">
+        <v>3</v>
+      </c>
+      <c r="O41" s="7">
+        <v>0</v>
+      </c>
+      <c r="P41" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="7">
+        <v>0</v>
+      </c>
+      <c r="R41" s="7">
+        <v>0</v>
+      </c>
+      <c r="S41" s="7">
+        <v>0</v>
+      </c>
+      <c r="T41" s="7">
+        <v>0</v>
+      </c>
+      <c r="U41" s="7">
+        <v>0</v>
+      </c>
+      <c r="V41" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W37" t="s">
+      <c r="W41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="X37" t="s">
+      <c r="X41" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Y41" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Z37">
+      <c r="Z41" s="7">
         <v>49904</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="AA41" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AB37" t="s">
+      <c r="AB41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AD37">
-        <v>0</v>
-      </c>
-      <c r="AE37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="AC41" s="7"/>
+      <c r="AD41" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>42100</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C42" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38">
-        <v>6</v>
-      </c>
-      <c r="I38">
-        <v>6</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="D42" s="7">
+        <v>2</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1</v>
+      </c>
+      <c r="H42" s="7">
+        <v>6</v>
+      </c>
+      <c r="I42" s="7">
+        <v>6</v>
+      </c>
+      <c r="J42" s="7">
+        <v>0</v>
+      </c>
+      <c r="K42" s="7">
+        <v>1</v>
+      </c>
+      <c r="L42" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <v>3</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="R38">
-        <v>0</v>
-      </c>
-      <c r="S38">
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
-      <c r="U38">
-        <v>0</v>
-      </c>
-      <c r="V38" t="s">
+      <c r="M42" s="7">
+        <v>0</v>
+      </c>
+      <c r="N42" s="7">
+        <v>3</v>
+      </c>
+      <c r="O42" s="7">
+        <v>0</v>
+      </c>
+      <c r="P42" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="7">
+        <v>0</v>
+      </c>
+      <c r="R42" s="7">
+        <v>0</v>
+      </c>
+      <c r="S42" s="7">
+        <v>0</v>
+      </c>
+      <c r="T42" s="7">
+        <v>0</v>
+      </c>
+      <c r="U42" s="7">
+        <v>0</v>
+      </c>
+      <c r="V42" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W38" t="s">
-        <v>6</v>
-      </c>
-      <c r="X38" t="s">
+      <c r="W42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X42" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y38" t="s">
+      <c r="Y42" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z38">
+      <c r="Z42" s="7">
         <v>49904</v>
       </c>
-      <c r="AA38" t="s">
+      <c r="AA42" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AB38" t="s">
+      <c r="AB42" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AD38">
-        <v>0</v>
-      </c>
-      <c r="AE38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="AC42" s="7"/>
+      <c r="AD42" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>47853</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B43" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C43" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s">
-        <v>2</v>
-      </c>
-      <c r="F39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>6</v>
-      </c>
-      <c r="I39">
-        <v>6</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
+      <c r="D43" s="7">
+        <v>2</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="7">
+        <v>1</v>
+      </c>
+      <c r="H43" s="7">
+        <v>6</v>
+      </c>
+      <c r="I43" s="7">
+        <v>6</v>
+      </c>
+      <c r="J43" s="7">
+        <v>0</v>
+      </c>
+      <c r="K43" s="7">
         <v>5</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L43" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>3</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39">
-        <v>0</v>
-      </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
-      <c r="V39" t="s">
+      <c r="M43" s="7">
+        <v>0</v>
+      </c>
+      <c r="N43" s="7">
+        <v>3</v>
+      </c>
+      <c r="O43" s="7">
+        <v>0</v>
+      </c>
+      <c r="P43" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="7">
+        <v>0</v>
+      </c>
+      <c r="R43" s="7">
+        <v>0</v>
+      </c>
+      <c r="S43" s="7">
+        <v>0</v>
+      </c>
+      <c r="T43" s="7">
+        <v>0</v>
+      </c>
+      <c r="U43" s="7">
+        <v>0</v>
+      </c>
+      <c r="V43" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W39" t="s">
+      <c r="W43" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="X39" t="s">
+      <c r="X43" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Y43" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z39">
+      <c r="Z43" s="7">
         <v>49904</v>
       </c>
-      <c r="AA39" t="s">
+      <c r="AA43" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AB39" t="s">
+      <c r="AB43" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AD39">
-        <v>0</v>
-      </c>
-      <c r="AE39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="AC43" s="7"/>
+      <c r="AD43" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>47741</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B44" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C44" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>2</v>
-      </c>
-      <c r="F40" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>6</v>
-      </c>
-      <c r="I40">
-        <v>6</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="D44" s="7">
+        <v>2</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="7">
+        <v>1</v>
+      </c>
+      <c r="H44" s="7">
+        <v>6</v>
+      </c>
+      <c r="I44" s="7">
+        <v>6</v>
+      </c>
+      <c r="J44" s="7">
+        <v>0</v>
+      </c>
+      <c r="K44" s="7">
+        <v>1</v>
+      </c>
+      <c r="L44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>3</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>0</v>
-      </c>
-      <c r="S40">
-        <v>0</v>
-      </c>
-      <c r="T40">
-        <v>0</v>
-      </c>
-      <c r="U40">
-        <v>0</v>
-      </c>
-      <c r="V40" t="s">
+      <c r="M44" s="7">
+        <v>0</v>
+      </c>
+      <c r="N44" s="7">
+        <v>3</v>
+      </c>
+      <c r="O44" s="7">
+        <v>0</v>
+      </c>
+      <c r="P44" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="7">
+        <v>0</v>
+      </c>
+      <c r="R44" s="7">
+        <v>0</v>
+      </c>
+      <c r="S44" s="7">
+        <v>0</v>
+      </c>
+      <c r="T44" s="7">
+        <v>0</v>
+      </c>
+      <c r="U44" s="7">
+        <v>0</v>
+      </c>
+      <c r="V44" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W40" t="s">
-        <v>6</v>
-      </c>
-      <c r="X40" t="s">
+      <c r="W44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X44" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Y44" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z40">
+      <c r="Z44" s="7">
         <v>49904</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AA44" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AB40" t="s">
+      <c r="AB44" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AD40">
-        <v>0</v>
-      </c>
-      <c r="AE40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="AC44" s="7"/>
+      <c r="AD44" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>49990</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B45" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C45" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>6</v>
-      </c>
-      <c r="I41">
-        <v>6</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="D45" s="7">
+        <v>2</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="7">
+        <v>1</v>
+      </c>
+      <c r="H45" s="7">
+        <v>6</v>
+      </c>
+      <c r="I45" s="7">
+        <v>6</v>
+      </c>
+      <c r="J45" s="7">
+        <v>0</v>
+      </c>
+      <c r="K45" s="7">
+        <v>1</v>
+      </c>
+      <c r="L45" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41">
-        <v>0</v>
-      </c>
-      <c r="S41">
-        <v>0</v>
-      </c>
-      <c r="T41">
-        <v>0</v>
-      </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-      <c r="V41" t="s">
+      <c r="M45" s="7">
+        <v>0</v>
+      </c>
+      <c r="N45" s="7">
+        <v>0</v>
+      </c>
+      <c r="O45" s="7">
+        <v>0</v>
+      </c>
+      <c r="P45" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="7">
+        <v>0</v>
+      </c>
+      <c r="R45" s="7">
+        <v>0</v>
+      </c>
+      <c r="S45" s="7">
+        <v>0</v>
+      </c>
+      <c r="T45" s="7">
+        <v>0</v>
+      </c>
+      <c r="U45" s="7">
+        <v>0</v>
+      </c>
+      <c r="V45" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Z41">
-        <v>0</v>
-      </c>
-      <c r="AD41">
-        <v>0</v>
-      </c>
-      <c r="AE41">
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
+      <c r="AC45" s="7"/>
+      <c r="AD45" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="7">
         <v>0</v>
       </c>
     </row>
@@ -4384,29 +4559,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>96</v>
       </c>

</xml_diff>